<commit_message>
Update output channels in Main.jl and adjust Results.jl inclusion
</commit_message>
<xml_diff>
--- a/results_presentation/UNet_Berechnen.xlsx
+++ b/results_presentation/UNet_Berechnen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Masterarbeit\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Masterarbeit\results_presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ED9A81-F79E-47C9-8827-CAAD37959846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E222B8-52BF-473B-9381-259480F9699F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17265" yWindow="1605" windowWidth="21600" windowHeight="11295" xr2:uid="{3538B6B0-B1DE-42DE-A4BF-20A52176B29F}"/>
+    <workbookView xWindow="2895" yWindow="1530" windowWidth="21600" windowHeight="11295" xr2:uid="{3538B6B0-B1DE-42DE-A4BF-20A52176B29F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>Stridehöhe</t>
   </si>
@@ -66,16 +66,58 @@
   </si>
   <si>
     <t>Dimension</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Epoche 1</t>
+  </si>
+  <si>
+    <t>Epoche 2</t>
+  </si>
+  <si>
+    <t>Epoche 3</t>
+  </si>
+  <si>
+    <t>Epoche 4</t>
+  </si>
+  <si>
+    <t>Epoche 5</t>
+  </si>
+  <si>
+    <t>Epoche 6</t>
+  </si>
+  <si>
+    <t>Epoche 7</t>
+  </si>
+  <si>
+    <t>Epoche 8</t>
+  </si>
+  <si>
+    <t>Epoche 9</t>
+  </si>
+  <si>
+    <t>Epoche 10</t>
+  </si>
+  <si>
+    <t>7h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,6 +160,946 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> Loss per Epoche</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$A$21:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Epoche 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Epoche 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Epoche 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Epoche 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Epoche 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Epoche 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Epoche 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Epoche 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Epoche 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Epoche 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$21:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>61.402850000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.540306000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.203457</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.548717000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.443863</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>57.139209999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56.979477000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56.936126999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.763170000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56.687477000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-728B-4D92-A90C-FE33657BC89F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1822540975"/>
+        <c:axId val="1822542895"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1822540975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1822542895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1822542895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1822540975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C3EAD63-C38A-D3CA-4999-33EF79183797}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14B8341-8BAF-45F6-AAC9-F238FA0AA158}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,26 +1639,118 @@
         <v>5.875</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>61.402850000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>58.540306000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>58.203457</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>57.548717000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>57.443863</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>57.139209999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>56.979477000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>56.936126999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>56.763170000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>56.687477000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="768ccc40-3631-450f-87b0-3142498a2bc0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="768ccc40-3631-450f-87b0-3142498a2bc0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -907,14 +1981,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19DE826-1672-41B5-8418-839BC21FE4A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{151798C9-BF44-400C-90BF-D6075FFBD701}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -927,6 +1993,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="4bbe938f-0039-42e7-aafe-6bba795bd972"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A19DE826-1672-41B5-8418-839BC21FE4A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>